<commit_message>
AI can build town on captured hexa
</commit_message>
<xml_diff>
--- a/AI.xlsx
+++ b/AI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>Město</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Points (1- obsaď hexu)</t>
+  </si>
+  <si>
+    <t>Posvatna hora</t>
+  </si>
+  <si>
+    <t>Capture</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:BW2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BW2" sqref="B2:BW2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="P1" t="s">
         <v>11</v>
@@ -603,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="AZ1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="BA1" t="s">
         <v>11</v>
@@ -676,11 +682,11 @@
       </c>
     </row>
     <row r="2" spans="1:75">
-      <c r="A2">
-        <v>8</v>
+      <c r="A2" t="s">
+        <v>28</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -698,7 +704,7 @@
         <v>10</v>
       </c>
       <c r="H2">
-        <v>250</v>
+        <v>20000</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -713,16 +719,16 @@
         <v>500</v>
       </c>
       <c r="M2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="N2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="P2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -809,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="AS2">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="AT2">
         <v>100</v>
@@ -821,19 +827,19 @@
         <v>0</v>
       </c>
       <c r="AW2">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="AX2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="AY2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AZ2">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="BA2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="BB2">
         <v>0</v>
@@ -890,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="BT2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU2">
         <v>0</v>

</xml_diff>

<commit_message>
AI for map 13 and 14
</commit_message>
<xml_diff>
--- a/AI.xlsx
+++ b/AI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t>Město</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Capture</t>
+  </si>
+  <si>
+    <t>Otto Sverdrup</t>
+  </si>
+  <si>
+    <t>Tom Crean</t>
+  </si>
+  <si>
+    <t>Helen Thayer</t>
   </si>
 </sst>
 </file>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BW2"/>
+  <dimension ref="A1:BW5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -905,6 +914,687 @@
         <v>400</v>
       </c>
       <c r="BW2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>350</v>
+      </c>
+      <c r="C3">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1200</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>5</v>
+      </c>
+      <c r="V3">
+        <v>90</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1600</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>5</v>
+      </c>
+      <c r="AB3">
+        <v>90</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>1200</v>
+      </c>
+      <c r="AF3">
+        <v>10</v>
+      </c>
+      <c r="AG3">
+        <v>300</v>
+      </c>
+      <c r="AH3">
+        <v>30</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>10</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>350</v>
+      </c>
+      <c r="AN3">
+        <v>60</v>
+      </c>
+      <c r="AO3">
+        <v>40</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>50</v>
+      </c>
+      <c r="AR3">
+        <v>10</v>
+      </c>
+      <c r="AS3">
+        <v>300</v>
+      </c>
+      <c r="AT3">
+        <v>10</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>90</v>
+      </c>
+      <c r="AW3">
+        <v>10</v>
+      </c>
+      <c r="AX3">
+        <v>30</v>
+      </c>
+      <c r="AY3">
+        <v>20</v>
+      </c>
+      <c r="AZ3">
+        <v>40</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
+        <v>100</v>
+      </c>
+      <c r="BE3">
+        <v>30</v>
+      </c>
+      <c r="BF3">
+        <v>10</v>
+      </c>
+      <c r="BG3">
+        <v>60</v>
+      </c>
+      <c r="BH3">
+        <v>0</v>
+      </c>
+      <c r="BI3">
+        <v>0</v>
+      </c>
+      <c r="BJ3">
+        <v>100</v>
+      </c>
+      <c r="BK3">
+        <v>10</v>
+      </c>
+      <c r="BL3">
+        <v>30</v>
+      </c>
+      <c r="BM3">
+        <v>60</v>
+      </c>
+      <c r="BN3">
+        <v>0</v>
+      </c>
+      <c r="BO3">
+        <v>0</v>
+      </c>
+      <c r="BP3">
+        <v>50</v>
+      </c>
+      <c r="BQ3">
+        <v>30</v>
+      </c>
+      <c r="BR3">
+        <v>50</v>
+      </c>
+      <c r="BS3">
+        <v>30</v>
+      </c>
+      <c r="BT3">
+        <v>0</v>
+      </c>
+      <c r="BU3">
+        <v>0</v>
+      </c>
+      <c r="BV3">
+        <v>10</v>
+      </c>
+      <c r="BW3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>350</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>80</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1200</v>
+      </c>
+      <c r="T4">
+        <v>5</v>
+      </c>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
+        <v>90</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>600</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
+        <v>5</v>
+      </c>
+      <c r="AB4">
+        <v>90</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>600</v>
+      </c>
+      <c r="AF4">
+        <v>10</v>
+      </c>
+      <c r="AG4">
+        <v>600</v>
+      </c>
+      <c r="AH4">
+        <v>30</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>10</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>350</v>
+      </c>
+      <c r="AN4">
+        <v>60</v>
+      </c>
+      <c r="AO4">
+        <v>40</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>50</v>
+      </c>
+      <c r="AR4">
+        <v>10</v>
+      </c>
+      <c r="AS4">
+        <v>300</v>
+      </c>
+      <c r="AT4">
+        <v>20</v>
+      </c>
+      <c r="AU4">
+        <v>80</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>100</v>
+      </c>
+      <c r="BE4">
+        <v>30</v>
+      </c>
+      <c r="BF4">
+        <v>10</v>
+      </c>
+      <c r="BG4">
+        <v>60</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>500</v>
+      </c>
+      <c r="BK4">
+        <v>10</v>
+      </c>
+      <c r="BL4">
+        <v>30</v>
+      </c>
+      <c r="BM4">
+        <v>60</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4">
+        <v>0</v>
+      </c>
+      <c r="BP4">
+        <v>500</v>
+      </c>
+      <c r="BQ4">
+        <v>30</v>
+      </c>
+      <c r="BR4">
+        <v>50</v>
+      </c>
+      <c r="BS4">
+        <v>30</v>
+      </c>
+      <c r="BT4">
+        <v>0</v>
+      </c>
+      <c r="BU4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>10</v>
+      </c>
+      <c r="BW4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>250</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>600</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>80</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>600</v>
+      </c>
+      <c r="T5">
+        <v>5</v>
+      </c>
+      <c r="U5">
+        <v>5</v>
+      </c>
+      <c r="V5">
+        <v>90</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>1600</v>
+      </c>
+      <c r="Z5">
+        <v>5</v>
+      </c>
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <v>90</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>1200</v>
+      </c>
+      <c r="AF5">
+        <v>10</v>
+      </c>
+      <c r="AG5">
+        <v>100</v>
+      </c>
+      <c r="AH5">
+        <v>30</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>10</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>350</v>
+      </c>
+      <c r="AN5">
+        <v>60</v>
+      </c>
+      <c r="AO5">
+        <v>40</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>50</v>
+      </c>
+      <c r="AR5">
+        <v>10</v>
+      </c>
+      <c r="AS5">
+        <v>300</v>
+      </c>
+      <c r="AT5">
+        <v>40</v>
+      </c>
+      <c r="AU5">
+        <v>60</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>60</v>
+      </c>
+      <c r="AX5">
+        <v>30</v>
+      </c>
+      <c r="AY5">
+        <v>20</v>
+      </c>
+      <c r="AZ5">
+        <v>40</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>500</v>
+      </c>
+      <c r="BE5">
+        <v>30</v>
+      </c>
+      <c r="BF5">
+        <v>10</v>
+      </c>
+      <c r="BG5">
+        <v>60</v>
+      </c>
+      <c r="BH5">
+        <v>0</v>
+      </c>
+      <c r="BI5">
+        <v>0</v>
+      </c>
+      <c r="BJ5">
+        <v>100</v>
+      </c>
+      <c r="BK5">
+        <v>10</v>
+      </c>
+      <c r="BL5">
+        <v>30</v>
+      </c>
+      <c r="BM5">
+        <v>60</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5">
+        <v>0</v>
+      </c>
+      <c r="BP5">
+        <v>50</v>
+      </c>
+      <c r="BQ5">
+        <v>30</v>
+      </c>
+      <c r="BR5">
+        <v>500</v>
+      </c>
+      <c r="BS5">
+        <v>30</v>
+      </c>
+      <c r="BT5">
+        <v>0</v>
+      </c>
+      <c r="BU5">
+        <v>0</v>
+      </c>
+      <c r="BV5">
+        <v>10</v>
+      </c>
+      <c r="BW5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AI building special building bug fixed
</commit_message>
<xml_diff>
--- a/AI.xlsx
+++ b/AI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="12435" windowHeight="5445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="12435" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="AI" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>Město</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Temné oči</t>
+  </si>
+  <si>
+    <t>Charles Wilkes</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BW9"/>
+  <dimension ref="A1:BW10"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BJ8" sqref="BJ8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2570,6 +2573,233 @@
       </c>
       <c r="BW9">
         <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>346</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>88</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>397</v>
+      </c>
+      <c r="G10">
+        <v>66</v>
+      </c>
+      <c r="H10">
+        <v>609</v>
+      </c>
+      <c r="I10">
+        <v>51</v>
+      </c>
+      <c r="J10">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>28</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1500</v>
+      </c>
+      <c r="T10">
+        <v>43</v>
+      </c>
+      <c r="U10">
+        <v>13</v>
+      </c>
+      <c r="V10">
+        <v>10</v>
+      </c>
+      <c r="W10">
+        <v>12</v>
+      </c>
+      <c r="X10">
+        <v>22</v>
+      </c>
+      <c r="Y10">
+        <v>500</v>
+      </c>
+      <c r="Z10">
+        <v>7</v>
+      </c>
+      <c r="AA10">
+        <v>46</v>
+      </c>
+      <c r="AB10">
+        <v>28</v>
+      </c>
+      <c r="AC10">
+        <v>15</v>
+      </c>
+      <c r="AD10">
+        <v>4</v>
+      </c>
+      <c r="AE10">
+        <v>338</v>
+      </c>
+      <c r="AF10">
+        <v>87</v>
+      </c>
+      <c r="AG10">
+        <v>535</v>
+      </c>
+      <c r="AH10">
+        <v>46</v>
+      </c>
+      <c r="AI10">
+        <v>11</v>
+      </c>
+      <c r="AJ10">
+        <v>73</v>
+      </c>
+      <c r="AK10">
+        <v>355</v>
+      </c>
+      <c r="AL10">
+        <v>85</v>
+      </c>
+      <c r="AM10">
+        <v>1000</v>
+      </c>
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <v>60</v>
+      </c>
+      <c r="AP10">
+        <v>39</v>
+      </c>
+      <c r="AQ10">
+        <v>971</v>
+      </c>
+      <c r="AR10">
+        <v>7</v>
+      </c>
+      <c r="AS10">
+        <v>10</v>
+      </c>
+      <c r="AT10">
+        <v>64</v>
+      </c>
+      <c r="AU10">
+        <v>18</v>
+      </c>
+      <c r="AV10">
+        <v>18</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>179</v>
+      </c>
+      <c r="BC10">
+        <v>20</v>
+      </c>
+      <c r="BD10">
+        <v>1800</v>
+      </c>
+      <c r="BE10">
+        <v>10</v>
+      </c>
+      <c r="BF10">
+        <v>10</v>
+      </c>
+      <c r="BG10">
+        <v>10</v>
+      </c>
+      <c r="BH10">
+        <v>10</v>
+      </c>
+      <c r="BI10">
+        <v>60</v>
+      </c>
+      <c r="BJ10">
+        <v>1800</v>
+      </c>
+      <c r="BK10">
+        <v>10</v>
+      </c>
+      <c r="BL10">
+        <v>10</v>
+      </c>
+      <c r="BM10">
+        <v>10</v>
+      </c>
+      <c r="BN10">
+        <v>10</v>
+      </c>
+      <c r="BO10">
+        <v>60</v>
+      </c>
+      <c r="BP10">
+        <v>3000</v>
+      </c>
+      <c r="BQ10">
+        <v>29</v>
+      </c>
+      <c r="BR10">
+        <v>3000</v>
+      </c>
+      <c r="BS10">
+        <v>61</v>
+      </c>
+      <c r="BT10">
+        <v>0</v>
+      </c>
+      <c r="BU10">
+        <v>0</v>
+      </c>
+      <c r="BV10">
+        <v>0</v>
+      </c>
+      <c r="BW10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2582,8 +2812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2603,20 +2833,41 @@
       <c r="A2" t="s">
         <v>40</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>41</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>42</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>43</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5">

</xml_diff>

<commit_message>
Materials hidden for other players
</commit_message>
<xml_diff>
--- a/AI.xlsx
+++ b/AI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="12435" windowHeight="5445"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="12435" windowHeight="5445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AI" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Město</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Charles Wilkes</t>
+  </si>
+  <si>
+    <t>Obtížnost</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2810,26 +2813,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2839,90 +2845,243 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>43</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>54</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2932,12 +3091,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="3:4">
+      <c r="C2" s="1">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4">
+      <c r="C3">
+        <v>802</v>
+      </c>
+      <c r="D3">
+        <f>C3-C2</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4">
+      <c r="C4">
+        <v>892</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="0">C4-C3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6">
+        <v>1178</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7">
+        <v>1334</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8">
+        <v>1449</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>